<commit_message>
Marketing Master Plan Checked In
Marketing Master Plan Checked In
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/CRM/Enquiry.xlsx
+++ b/Offline/BusinessManagement/CRM/Enquiry.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\CRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F386AE1-A498-4011-8346-BF622FDB9205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E98F9B-9C87-4A49-A562-AD738DA99A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Students-Prospects" sheetId="2" r:id="rId2"/>
     <sheet name="Daily-Visit" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="181">
   <si>
     <t>Student Name</t>
   </si>
@@ -555,6 +556,21 @@
   </si>
   <si>
     <t>Gopal Mondal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seminar Date </t>
+  </si>
+  <si>
+    <t>Seminar Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student </t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Gurdian</t>
   </si>
 </sst>
 </file>
@@ -4150,7 +4166,7 @@
   <dimension ref="A1:O59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5965,10 +5981,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECF2424-D6E5-483B-A49D-6898AA1F3E64}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5983,9 +5999,10 @@
     <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="75.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>127</v>
       </c>
@@ -6017,10 +6034,19 @@
         <v>133</v>
       </c>
       <c r="K1" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="M1" s="16" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N1" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="17">
         <v>1</v>
       </c>
@@ -6043,7 +6069,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="17">
         <v>2</v>
       </c>
@@ -6054,7 +6080,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
         <v>3</v>
       </c>
@@ -6074,7 +6100,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" s="15"/>
       <c r="E5" t="s">
         <v>140</v>
@@ -6089,7 +6115,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>144</v>
       </c>
@@ -6106,7 +6132,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <v>4</v>
       </c>
@@ -6126,7 +6152,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
         <v>5</v>
       </c>
@@ -6140,7 +6166,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
         <v>6</v>
       </c>
@@ -6163,7 +6189,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="17">
         <v>7</v>
       </c>
@@ -6180,7 +6206,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="17">
         <v>8</v>
       </c>
@@ -6197,7 +6223,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="17">
         <v>9</v>
       </c>
@@ -6214,7 +6240,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <v>10</v>
       </c>
@@ -6231,7 +6257,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>11</v>
       </c>
@@ -6251,7 +6277,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="17">
         <v>12</v>
       </c>
@@ -6268,7 +6294,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="17">
         <v>13</v>
       </c>
@@ -6368,6 +6394,44 @@
       </c>
       <c r="D21">
         <v>9064573012</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9BE59D4-FD08-4612-851B-E358E933A94E}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mock Test Queries checked in
Mock Test Queries checked in
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/CRM/Enquiry.xlsx
+++ b/Offline/BusinessManagement/CRM/Enquiry.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\CRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050B7DCF-64D0-4A05-BBD9-60ADF1CDC354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873097A3-EE2D-41C0-BB8A-76F7689F1D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New-Prospects" sheetId="6" r:id="rId1"/>
     <sheet name="Old-Prospects" sheetId="2" r:id="rId2"/>
     <sheet name="Seminar-Plan" sheetId="5" r:id="rId3"/>
+    <sheet name="Daily-Marketing-Plan" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -1055,7 +1056,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1124,9 +1125,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1161,8 +1159,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1480,7 +1478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
@@ -1555,34 +1553,34 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27">
+      <c r="A3" s="26">
         <v>2</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="27">
         <v>45246</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="28" t="s">
         <v>267</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="29">
+      <c r="D3" s="26"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="28">
         <v>9830610602</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="28" t="s">
         <v>240</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="28" t="s">
         <v>266</v>
       </c>
-      <c r="I3" s="31" t="s">
+      <c r="I3" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="J3" s="31"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="30"/>
+      <c r="K3" s="31" t="s">
         <v>259</v>
       </c>
-      <c r="L3" s="31" t="s">
+      <c r="L3" s="30" t="s">
         <v>258</v>
       </c>
     </row>
@@ -1590,63 +1588,63 @@
       <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="35">
+      <c r="B4" s="34">
         <v>45246</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="35" t="s">
         <v>238</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="38" t="s">
+      <c r="D4" s="33"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="37" t="s">
         <v>239</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="H4" s="35" t="s">
         <v>265</v>
       </c>
-      <c r="I4" s="39" t="s">
+      <c r="I4" s="38" t="s">
         <v>244</v>
       </c>
-      <c r="J4" s="39"/>
-      <c r="K4" s="40" t="s">
+      <c r="J4" s="38"/>
+      <c r="K4" s="39" t="s">
         <v>261</v>
       </c>
-      <c r="L4" s="39" t="s">
+      <c r="L4" s="38" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="27">
+      <c r="A5" s="26">
         <v>4</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="27">
         <v>45246</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>242</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="33" t="s">
+      <c r="D5" s="26"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="28" t="s">
         <v>257</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="28" t="s">
         <v>266</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="32" t="s">
+      <c r="J5" s="30"/>
+      <c r="K5" s="31" t="s">
         <v>259</v>
       </c>
-      <c r="L5" s="31" t="s">
+      <c r="L5" s="30" t="s">
         <v>258</v>
       </c>
     </row>
@@ -1680,7 +1678,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="41">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="9">
@@ -1738,7 +1736,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="41">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="9">
@@ -1773,7 +1771,7 @@
       <c r="F10" s="23"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="41">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="9">
@@ -5261,10 +5259,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="26"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
@@ -5721,4 +5719,18 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16512463-536B-4DEE-86DA-9893C0832B07}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mock Test Queries Updated
Mock Test Queries Updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/CRM/Enquiry.xlsx
+++ b/Offline/BusinessManagement/CRM/Enquiry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\CRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873097A3-EE2D-41C0-BB8A-76F7689F1D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977F85F4-7786-48D6-BC82-5BE4BB696121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New-Prospects" sheetId="6" r:id="rId1"/>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="271">
   <si>
     <t>Student Name</t>
   </si>
@@ -933,6 +933,15 @@
   </si>
   <si>
     <t>Ayushman  Sarkar</t>
+  </si>
+  <si>
+    <t>Ishan Kumar</t>
+  </si>
+  <si>
+    <t>7449868584</t>
+  </si>
+  <si>
+    <t>All Subjects</t>
   </si>
 </sst>
 </file>
@@ -1478,8 +1487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1783,7 +1792,25 @@
       <c r="F11" s="23"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
       <c r="B12" s="1"/>
+      <c r="C12" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>245</v>
+      </c>
+      <c r="J12" t="s">
+        <v>270</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
@@ -2618,7 +2645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A121" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -5725,7 +5752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16512463-536B-4DEE-86DA-9893C0832B07}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
UPDATED CRM CALLS AS ON 01.12.23
UPDATED CRM CALLS AS ON 01.12.23
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/CRM/Enquiry.xlsx
+++ b/Offline/BusinessManagement/CRM/Enquiry.xlsx
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="273">
   <si>
     <t>Student Name</t>
   </si>
@@ -966,6 +966,48 @@
   </si>
   <si>
     <t>DIDN’T PICK UP</t>
+  </si>
+  <si>
+    <t>DIDN’T PICKUP CALL</t>
+  </si>
+  <si>
+    <t>INVALID</t>
+  </si>
+  <si>
+    <t>SWITCHED OFF</t>
+  </si>
+  <si>
+    <t>9 DIGIT NUMBER</t>
+  </si>
+  <si>
+    <t>NOT INTERSTED</t>
+  </si>
+  <si>
+    <t>SPECIAL CHILD</t>
+  </si>
+  <si>
+    <t>NOT INTERESTED</t>
+  </si>
+  <si>
+    <t>POTENTIAL</t>
+  </si>
+  <si>
+    <t>BUSY</t>
+  </si>
+  <si>
+    <t>INTERSTED</t>
+  </si>
+  <si>
+    <t>will call us LATER</t>
+  </si>
+  <si>
+    <t>NEXT YEAR</t>
+  </si>
+  <si>
+    <t>CARE-TAKERS NUMBER</t>
+  </si>
+  <si>
+    <t>WILL COME TO OUR OFFICE</t>
   </si>
 </sst>
 </file>
@@ -3111,8 +3153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="J78" sqref="J78"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="J102" sqref="J102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4667,6 +4709,9 @@
         <v>132</v>
       </c>
       <c r="I78"/>
+      <c r="J78" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" s="1">
@@ -4686,6 +4731,9 @@
         <v>132</v>
       </c>
       <c r="I79"/>
+      <c r="J79" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="1">
@@ -4705,8 +4753,11 @@
         <v>132</v>
       </c>
       <c r="I80"/>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="J80" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -4724,8 +4775,11 @@
         <v>132</v>
       </c>
       <c r="I81"/>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="J81" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -4743,8 +4797,11 @@
         <v>132</v>
       </c>
       <c r="I82"/>
-    </row>
-    <row r="83" spans="1:9">
+      <c r="J82" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -4762,8 +4819,11 @@
         <v>132</v>
       </c>
       <c r="I83"/>
-    </row>
-    <row r="84" spans="1:9">
+      <c r="J83" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -4781,8 +4841,11 @@
         <v>134</v>
       </c>
       <c r="I84"/>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="J84" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -4800,8 +4863,11 @@
         <v>134</v>
       </c>
       <c r="I85"/>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="J85" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -4819,8 +4885,11 @@
         <v>134</v>
       </c>
       <c r="I86"/>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="J86" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -4838,8 +4907,11 @@
         <v>134</v>
       </c>
       <c r="I87"/>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="J87" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -4857,8 +4929,11 @@
         <v>134</v>
       </c>
       <c r="I88"/>
-    </row>
-    <row r="89" spans="1:9">
+      <c r="J88" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -4876,8 +4951,11 @@
         <v>134</v>
       </c>
       <c r="I89"/>
-    </row>
-    <row r="90" spans="1:9">
+      <c r="J89" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -4895,8 +4973,11 @@
         <v>134</v>
       </c>
       <c r="I90"/>
-    </row>
-    <row r="91" spans="1:9">
+      <c r="J90" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -4914,8 +4995,11 @@
         <v>134</v>
       </c>
       <c r="I91"/>
-    </row>
-    <row r="92" spans="1:9">
+      <c r="J91" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -4933,8 +5017,11 @@
         <v>134</v>
       </c>
       <c r="I92"/>
-    </row>
-    <row r="93" spans="1:9">
+      <c r="J92" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -4952,8 +5039,11 @@
         <v>134</v>
       </c>
       <c r="I93"/>
-    </row>
-    <row r="94" spans="1:9">
+      <c r="J93" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -4971,8 +5061,11 @@
         <v>134</v>
       </c>
       <c r="I94"/>
-    </row>
-    <row r="95" spans="1:9">
+      <c r="J94" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -4990,8 +5083,11 @@
         <v>134</v>
       </c>
       <c r="I95"/>
-    </row>
-    <row r="96" spans="1:9">
+      <c r="J95" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -5009,8 +5105,11 @@
         <v>142</v>
       </c>
       <c r="I96"/>
-    </row>
-    <row r="97" spans="1:9">
+      <c r="J96" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -5028,8 +5127,11 @@
         <v>142</v>
       </c>
       <c r="I97"/>
-    </row>
-    <row r="98" spans="1:9">
+      <c r="J97" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -5047,8 +5149,11 @@
         <v>142</v>
       </c>
       <c r="I98"/>
-    </row>
-    <row r="99" spans="1:9">
+      <c r="J98" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -5066,8 +5171,11 @@
         <v>145</v>
       </c>
       <c r="I99"/>
-    </row>
-    <row r="100" spans="1:9">
+      <c r="J99" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -5085,8 +5193,11 @@
         <v>145</v>
       </c>
       <c r="I100"/>
-    </row>
-    <row r="101" spans="1:9">
+      <c r="J100" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -5104,8 +5215,11 @@
         <v>145</v>
       </c>
       <c r="I101"/>
-    </row>
-    <row r="102" spans="1:9">
+      <c r="J101" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -5124,7 +5238,7 @@
       </c>
       <c r="I102"/>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:10">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -5143,7 +5257,7 @@
       </c>
       <c r="I103"/>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:10">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -5162,7 +5276,7 @@
       </c>
       <c r="I104"/>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:10">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -5181,7 +5295,7 @@
       </c>
       <c r="I105"/>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:10">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -5200,7 +5314,7 @@
       </c>
       <c r="I106"/>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:10">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -5219,7 +5333,7 @@
       </c>
       <c r="I107"/>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:10">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -5238,7 +5352,7 @@
       </c>
       <c r="I108"/>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:10">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -5257,7 +5371,7 @@
       </c>
       <c r="I109"/>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:10">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -5276,7 +5390,7 @@
       </c>
       <c r="I110"/>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:10">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -5295,7 +5409,7 @@
       </c>
       <c r="I111"/>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:10">
       <c r="A112" s="1">
         <v>110</v>
       </c>

</xml_diff>

<commit_message>
CRM sheet for Rahul is done
CRM sheet for Rahul is done
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/CRM/Enquiry.xlsx
+++ b/Offline/BusinessManagement/CRM/Enquiry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\CRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7B3C08-FCC7-4369-AA3F-0C4859D9E00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0105A05B-CB6A-4FC0-863C-312668556FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="437" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="437" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prospects" sheetId="2" r:id="rId1"/>
@@ -1274,7 +1274,7 @@
       <name val="Oxygen"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1295,12 +1295,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1314,24 +1308,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1424,7 +1400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1460,10 +1436,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1481,7 +1457,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1524,6 +1500,20 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1531,36 +1521,16 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1587,6 +1557,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1983,8 +1954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O497"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
@@ -6575,28 +6546,28 @@
       <c r="A139" s="6">
         <v>138</v>
       </c>
-      <c r="B139" s="60">
+      <c r="B139" s="54">
         <v>45246</v>
       </c>
-      <c r="C139" s="60">
+      <c r="C139" s="54">
         <v>45246</v>
       </c>
-      <c r="D139" s="61" t="s">
+      <c r="D139" s="55" t="s">
         <v>203</v>
       </c>
-      <c r="E139" s="62"/>
-      <c r="F139" s="63"/>
-      <c r="G139" s="64"/>
-      <c r="H139" s="64"/>
-      <c r="I139" s="65"/>
-      <c r="J139" s="65"/>
-      <c r="K139" s="63"/>
-      <c r="L139" s="63"/>
-      <c r="M139" s="65"/>
-      <c r="N139" s="66" t="s">
-        <v>210</v>
-      </c>
-      <c r="O139" s="65" t="s">
+      <c r="E139" s="56"/>
+      <c r="F139" s="57"/>
+      <c r="G139" s="58"/>
+      <c r="H139" s="58"/>
+      <c r="I139" s="59"/>
+      <c r="J139" s="59"/>
+      <c r="K139" s="57"/>
+      <c r="L139" s="57"/>
+      <c r="M139" s="59"/>
+      <c r="N139" s="60" t="s">
+        <v>210</v>
+      </c>
+      <c r="O139" s="59" t="s">
         <v>256</v>
       </c>
     </row>
@@ -6604,28 +6575,28 @@
       <c r="A140" s="6">
         <v>139</v>
       </c>
-      <c r="B140" s="60">
+      <c r="B140" s="54">
         <v>45246</v>
       </c>
-      <c r="C140" s="60">
+      <c r="C140" s="54">
         <v>45246</v>
       </c>
-      <c r="D140" s="61" t="s">
+      <c r="D140" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="E140" s="62"/>
-      <c r="F140" s="63"/>
-      <c r="G140" s="64"/>
-      <c r="H140" s="64"/>
-      <c r="I140" s="65"/>
-      <c r="J140" s="65"/>
-      <c r="K140" s="63"/>
-      <c r="L140" s="63"/>
-      <c r="M140" s="65"/>
-      <c r="N140" s="66" t="s">
-        <v>210</v>
-      </c>
-      <c r="O140" s="65" t="s">
+      <c r="E140" s="56"/>
+      <c r="F140" s="57"/>
+      <c r="G140" s="58"/>
+      <c r="H140" s="58"/>
+      <c r="I140" s="59"/>
+      <c r="J140" s="59"/>
+      <c r="K140" s="57"/>
+      <c r="L140" s="57"/>
+      <c r="M140" s="59"/>
+      <c r="N140" s="60" t="s">
+        <v>210</v>
+      </c>
+      <c r="O140" s="59" t="s">
         <v>256</v>
       </c>
     </row>
@@ -13072,8 +13043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF1703B3-076E-40BB-A643-6D0582148E8C}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13087,15 +13058,15 @@
       <c r="A1" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="61" t="s">
         <v>259</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="69"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
@@ -13129,7 +13100,7 @@
       <c r="B5" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="64" t="s">
         <v>257</v>
       </c>
     </row>
@@ -13140,7 +13111,7 @@
       <c r="B6" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="64" t="s">
         <v>211</v>
       </c>
     </row>
@@ -13151,7 +13122,7 @@
       <c r="B7" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="64" t="s">
         <v>284</v>
       </c>
     </row>
@@ -13162,7 +13133,7 @@
       <c r="B8" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="64" t="s">
         <v>285</v>
       </c>
     </row>
@@ -13173,7 +13144,7 @@
       <c r="B9" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="64" t="s">
         <v>286</v>
       </c>
     </row>
@@ -13184,7 +13155,7 @@
       <c r="B10" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="64" t="s">
         <v>256</v>
       </c>
     </row>
@@ -13195,7 +13166,7 @@
       <c r="B11" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="64" t="s">
         <v>255</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Payout Slips for Nov 2023
Payout Slips for Nov 2023 done
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/CRM/Enquiry.xlsx
+++ b/Offline/BusinessManagement/CRM/Enquiry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\CRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1B2AC8-03D6-452C-9A31-369E6421ADE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF0D0F3-0BB4-4A48-8038-723D5B1637AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="437" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,6 +84,8 @@
     <author>tc={E5EF2C76-FFB2-45EA-B6C8-EC9A972B960A}</author>
     <author>tc={BD936E28-6500-430E-896F-A137AE40CCEB}</author>
     <author>tc={FF826963-E66D-4675-BE00-0061E3C0FE87}</author>
+    <author>tc={6688DD1B-E8EA-494F-A88B-321A8C0C2316}</author>
+    <author>tc={FC7F6E60-534C-43E8-9142-136010B706D4}</author>
   </authors>
   <commentList>
     <comment ref="M62" authorId="0" shapeId="0" xr:uid="{B4F983C8-7CA2-499B-9BA2-EE1FF232C344}">
@@ -487,12 +489,29 @@
 Follow-up date: 07-12-2023.</t>
       </text>
     </comment>
+    <comment ref="M160" authorId="44" shapeId="0" xr:uid="{6688DD1B-E8EA-494F-A88B-321A8C0C2316}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Right now her son will give final exam in Feb 2024, hence we will followup on 1st March 2024</t>
+      </text>
+    </comment>
+    <comment ref="M161" authorId="45" shapeId="0" xr:uid="{FC7F6E60-534C-43E8-9142-136010B706D4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    She did not take interest to join the course.
+Next Follow-Up Date : 11-12-2023.</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="318">
   <si>
     <t>Student Name</t>
   </si>
@@ -1442,17 +1461,17 @@
     <t>Rina Dey Ganguly</t>
   </si>
   <si>
-    <t>Std XI</t>
-  </si>
-  <si>
     <t>Commerce All Subjects ISC</t>
+  </si>
+  <si>
+    <t>Sreya Naskar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1482,6 +1501,12 @@
     <font>
       <sz val="10"/>
       <name val="Oxygen"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1765,6 +1790,9 @@
     <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1773,9 +1801,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2244,6 +2269,13 @@
 We need to tell him the course fee.
 Follow-up date: 07-12-2023.</text>
   </threadedComment>
+  <threadedComment ref="M160" dT="2023-12-08T09:32:06.09" personId="{4666E732-BD10-4E5E-A636-505584664154}" id="{6688DD1B-E8EA-494F-A88B-321A8C0C2316}">
+    <text>Right now her son will give final exam in Feb 2024, hence we will followup on 1st March 2024</text>
+  </threadedComment>
+  <threadedComment ref="M161" dT="2023-12-08T07:38:28.78" personId="{4666E732-BD10-4E5E-A636-505584664154}" id="{FC7F6E60-534C-43E8-9142-136010B706D4}">
+    <text>She did not take interest to join the course.
+Next Follow-Up Date : 11-12-2023.</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2251,9 +2283,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O494"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H140" sqref="H140"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M160" sqref="M160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6902,10 +6934,10 @@
       </c>
       <c r="E139" s="56"/>
       <c r="F139" s="25"/>
-      <c r="G139" s="67" t="s">
+      <c r="G139" s="64" t="s">
         <v>212</v>
       </c>
-      <c r="H139" s="67"/>
+      <c r="H139" s="64"/>
       <c r="I139" s="58"/>
       <c r="J139" s="8" t="s">
         <v>156</v>
@@ -7191,7 +7223,7 @@
       </c>
     </row>
     <row r="148" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="6">
+      <c r="A148" s="37">
         <v>147</v>
       </c>
       <c r="B148" s="38">
@@ -7226,7 +7258,7 @@
       </c>
     </row>
     <row r="149" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A149" s="6">
+      <c r="A149" s="37">
         <v>148</v>
       </c>
       <c r="B149" s="38">
@@ -7261,7 +7293,7 @@
       </c>
     </row>
     <row r="150" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A150" s="6">
+      <c r="A150" s="37">
         <v>149</v>
       </c>
       <c r="B150" s="38">
@@ -7296,7 +7328,7 @@
       </c>
     </row>
     <row r="151" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="6">
+      <c r="A151" s="37">
         <v>150</v>
       </c>
       <c r="B151" s="59">
@@ -7335,7 +7367,7 @@
       </c>
     </row>
     <row r="152" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A152" s="6">
+      <c r="A152" s="37">
         <v>151</v>
       </c>
       <c r="B152" s="38">
@@ -7370,7 +7402,7 @@
       </c>
     </row>
     <row r="153" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A153" s="6">
+      <c r="A153" s="37">
         <v>152</v>
       </c>
       <c r="B153" s="38">
@@ -7407,7 +7439,7 @@
       </c>
     </row>
     <row r="154" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A154" s="6">
+      <c r="A154" s="37">
         <v>153</v>
       </c>
       <c r="B154" s="38">
@@ -7442,7 +7474,7 @@
       </c>
     </row>
     <row r="155" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A155" s="6">
+      <c r="A155" s="37">
         <v>154</v>
       </c>
       <c r="B155" s="38">
@@ -7477,7 +7509,7 @@
       </c>
     </row>
     <row r="156" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A156" s="6">
+      <c r="A156" s="37">
         <v>155</v>
       </c>
       <c r="B156" s="38">
@@ -7510,7 +7542,7 @@
       </c>
     </row>
     <row r="157" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A157" s="6">
+      <c r="A157" s="37">
         <v>156</v>
       </c>
       <c r="B157" s="38">
@@ -7547,7 +7579,7 @@
       </c>
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A158" s="6">
+      <c r="A158" s="37">
         <v>157</v>
       </c>
       <c r="B158" s="38">
@@ -7580,7 +7612,7 @@
       </c>
     </row>
     <row r="159" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A159" s="6">
+      <c r="A159" s="37">
         <v>158</v>
       </c>
       <c r="B159" s="38">
@@ -7626,7 +7658,7 @@
         <v>315</v>
       </c>
       <c r="E160" s="18">
-        <v>9945738690</v>
+        <v>8240930263</v>
       </c>
       <c r="F160" s="15"/>
       <c r="G160" s="22"/>
@@ -7636,31 +7668,51 @@
         <v>156</v>
       </c>
       <c r="K160" s="17" t="s">
+        <v>316</v>
+      </c>
+      <c r="L160" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="M160" s="15"/>
+      <c r="N160" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="O160" s="15" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A161" s="23">
+        <v>160</v>
+      </c>
+      <c r="B161" s="20">
+        <v>45268</v>
+      </c>
+      <c r="C161" s="20">
+        <v>45268</v>
+      </c>
+      <c r="D161" s="17" t="s">
         <v>317</v>
       </c>
-      <c r="L160" s="17" t="s">
-        <v>316</v>
-      </c>
-      <c r="M160" s="15"/>
-      <c r="N160" s="16"/>
-      <c r="O160" s="15"/>
-    </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A161" s="23"/>
-      <c r="B161" s="15"/>
-      <c r="C161" s="15"/>
-      <c r="D161" s="17"/>
-      <c r="E161" s="18"/>
+      <c r="E161" s="18">
+        <v>7439626395</v>
+      </c>
       <c r="F161" s="15"/>
       <c r="G161" s="22"/>
       <c r="H161" s="19"/>
       <c r="I161" s="15"/>
-      <c r="J161" s="15"/>
-      <c r="K161" s="17"/>
+      <c r="J161" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="K161" s="17" t="s">
+        <v>289</v>
+      </c>
       <c r="L161" s="17"/>
       <c r="M161" s="15"/>
       <c r="N161" s="16"/>
-      <c r="O161" s="15"/>
+      <c r="O161" s="15" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="162" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A162" s="23"/>
@@ -13360,15 +13412,15 @@
       <c r="A1" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="65" t="s">
         <v>252</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="67"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="13">

</xml_diff>

<commit_message>
Excel sheet for demo on 16-12-2023 is created
Excel sheet for demo on 16-12-2023 is created
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/CRM/Enquiry.xlsx
+++ b/Offline/BusinessManagement/CRM/Enquiry.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\CRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E137021B-696D-4496-9227-FCEBFA392261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CAA700-13C0-48B7-99E3-3D37248A0F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="437" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="437" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prospects" sheetId="2" r:id="rId1"/>
-    <sheet name="Notes" sheetId="7" r:id="rId2"/>
+    <sheet name="Demo-16-12-2023" sheetId="8" r:id="rId2"/>
+    <sheet name="Notes" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Prospects!$A$1:$O$159</definedName>
@@ -75,6 +76,7 @@
     <author>tc={588025E0-A0E6-4E4A-9495-C2EA9C676DAF}</author>
     <author>tc={006DA87C-A4D4-4EB6-A53D-8225376469C4}</author>
     <author>tc={D7894310-9964-4FB2-B7D2-921476547B87}</author>
+    <author>tc={3937279E-0182-40B8-9848-6101AC89C064}</author>
     <author>tc={9F686F59-C29D-4D23-A297-DDD8C911F41F}</author>
     <author>tc={06C1A770-BDC3-4EE1-B6FA-36CCC1AAF8F9}</author>
     <author>tc={2358E5BF-6CE9-4B18-A908-A65F44178D1C}</author>
@@ -407,7 +409,15 @@
 </t>
       </text>
     </comment>
-    <comment ref="M149" authorId="35" shapeId="0" xr:uid="{9F686F59-C29D-4D23-A297-DDD8C911F41F}">
+    <comment ref="M148" authorId="35" shapeId="0" xr:uid="{3937279E-0182-40B8-9848-6101AC89C064}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Need to call as they are not picking up the call.</t>
+      </text>
+    </comment>
+    <comment ref="M149" authorId="36" shapeId="0" xr:uid="{9F686F59-C29D-4D23-A297-DDD8C911F41F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -415,16 +425,17 @@
     He is a retired person and he is keen to study computer course. Needs to follow up  on 07-12-2023 (Thursday).</t>
       </text>
     </comment>
-    <comment ref="M151" authorId="36" shapeId="0" xr:uid="{06C1A770-BDC3-4EE1-B6FA-36CCC1AAF8F9}">
+    <comment ref="M151" authorId="37" shapeId="0" xr:uid="{06C1A770-BDC3-4EE1-B6FA-36CCC1AAF8F9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Student is interested in vehicles. We can show robotics vehicles by Bappadito.
+    Needed to again call for demo.
+Student is interested in vehicles. We can show robotics vehicles by Bappadito.
 Demo class by Bappadito</t>
       </text>
     </comment>
-    <comment ref="M152" authorId="37" shapeId="0" xr:uid="{2358E5BF-6CE9-4B18-A908-A65F44178D1C}">
+    <comment ref="M152" authorId="38" shapeId="0" xr:uid="{2358E5BF-6CE9-4B18-A908-A65F44178D1C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -432,7 +443,7 @@
     She is a working lady. Follow up date 05-12-2023.</t>
       </text>
     </comment>
-    <comment ref="M153" authorId="38" shapeId="0" xr:uid="{020F2CA3-F192-4B9F-9B7D-1B455CAC0BBB}">
+    <comment ref="M153" authorId="39" shapeId="0" xr:uid="{020F2CA3-F192-4B9F-9B7D-1B455CAC0BBB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -440,7 +451,7 @@
     His daughter studies in GD Birla in class IX.She needs coaching in Physics.</t>
       </text>
     </comment>
-    <comment ref="M154" authorId="39" shapeId="0" xr:uid="{C0727A5B-EA0D-417C-9E76-E2B8CDF1AB5A}">
+    <comment ref="M154" authorId="40" shapeId="0" xr:uid="{C0727A5B-EA0D-417C-9E76-E2B8CDF1AB5A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -449,7 +460,7 @@
 She needs to be followed up on 06-12-2023.</t>
       </text>
     </comment>
-    <comment ref="M155" authorId="40" shapeId="0" xr:uid="{59D2B255-7D2E-4587-B857-CF4F4991A1B9}">
+    <comment ref="M155" authorId="41" shapeId="0" xr:uid="{59D2B255-7D2E-4587-B857-CF4F4991A1B9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -457,7 +468,7 @@
     His son can give mock test</t>
       </text>
     </comment>
-    <comment ref="M156" authorId="41" shapeId="0" xr:uid="{E5EF2C76-FFB2-45EA-B6C8-EC9A972B960A}">
+    <comment ref="M156" authorId="42" shapeId="0" xr:uid="{E5EF2C76-FFB2-45EA-B6C8-EC9A972B960A}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -466,7 +477,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="M157" authorId="42" shapeId="0" xr:uid="{BD936E28-6500-430E-896F-A137AE40CCEB}">
+    <comment ref="M157" authorId="43" shapeId="0" xr:uid="{BD936E28-6500-430E-896F-A137AE40CCEB}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -479,7 +490,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="M159" authorId="43" shapeId="0" xr:uid="{FF826963-E66D-4675-BE00-0061E3C0FE87}">
+    <comment ref="M159" authorId="44" shapeId="0" xr:uid="{FF826963-E66D-4675-BE00-0061E3C0FE87}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -489,7 +500,7 @@
 Follow-up date: 07-12-2023.</t>
       </text>
     </comment>
-    <comment ref="M160" authorId="44" shapeId="0" xr:uid="{6688DD1B-E8EA-494F-A88B-321A8C0C2316}">
+    <comment ref="M160" authorId="45" shapeId="0" xr:uid="{6688DD1B-E8EA-494F-A88B-321A8C0C2316}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -497,7 +508,7 @@
     Right now her son will give final exam in Feb 2024, hence we will followup on 1st March 2024</t>
       </text>
     </comment>
-    <comment ref="M161" authorId="45" shapeId="0" xr:uid="{FC7F6E60-534C-43E8-9142-136010B706D4}">
+    <comment ref="M161" authorId="46" shapeId="0" xr:uid="{FC7F6E60-534C-43E8-9142-136010B706D4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -511,7 +522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="318">
   <si>
     <t>Student Name</t>
   </si>
@@ -1471,7 +1482,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1501,6 +1512,12 @@
     <font>
       <sz val="10"/>
       <name val="Oxygen"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1623,7 +1640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1787,6 +1804,15 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1796,14 +1822,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2235,11 +2282,15 @@
     <text xml:space="preserve">All Subjects
 </text>
   </threadedComment>
+  <threadedComment ref="M148" dT="2023-12-09T05:49:44.22" personId="{4666E732-BD10-4E5E-A636-505584664154}" id="{3937279E-0182-40B8-9848-6101AC89C064}">
+    <text>Need to call as they are not picking up the call.</text>
+  </threadedComment>
   <threadedComment ref="M149" dT="2023-12-05T07:55:10.74" personId="{4666E732-BD10-4E5E-A636-505584664154}" id="{9F686F59-C29D-4D23-A297-DDD8C911F41F}">
     <text>He is a retired person and he is keen to study computer course. Needs to follow up  on 07-12-2023 (Thursday).</text>
   </threadedComment>
   <threadedComment ref="M151" dT="2023-12-04T08:10:56.08" personId="{4666E732-BD10-4E5E-A636-505584664154}" id="{06C1A770-BDC3-4EE1-B6FA-36CCC1AAF8F9}">
-    <text>Student is interested in vehicles. We can show robotics vehicles by Bappadito.
+    <text>Needed to again call for demo.
+Student is interested in vehicles. We can show robotics vehicles by Bappadito.
 Demo class by Bappadito</text>
   </threadedComment>
   <threadedComment ref="M152" dT="2023-12-05T06:38:50.42" personId="{4666E732-BD10-4E5E-A636-505584664154}" id="{2358E5BF-6CE9-4B18-A908-A65F44178D1C}">
@@ -2286,9 +2337,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O494"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M150" sqref="M150"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K162" sqref="K162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6763,23 +6814,23 @@
         <v>45246</v>
       </c>
       <c r="C134" s="38">
-        <v>45246</v>
+        <v>45268</v>
       </c>
       <c r="D134" s="60" t="s">
         <v>263</v>
       </c>
       <c r="E134" s="43"/>
-      <c r="F134" s="69" t="s">
+      <c r="F134" s="66" t="s">
         <v>264</v>
       </c>
-      <c r="G134" s="70" t="s">
+      <c r="G134" s="67" t="s">
         <v>194</v>
       </c>
-      <c r="H134" s="70"/>
-      <c r="I134" s="69" t="s">
+      <c r="H134" s="67"/>
+      <c r="I134" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="J134" s="69" t="s">
+      <c r="J134" s="66" t="s">
         <v>156</v>
       </c>
       <c r="K134" s="62" t="s">
@@ -6791,7 +6842,7 @@
         <v>205</v>
       </c>
       <c r="O134" s="62" t="s">
-        <v>250</v>
+        <v>206</v>
       </c>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.3">
@@ -6802,21 +6853,21 @@
         <v>45246</v>
       </c>
       <c r="C135" s="38">
-        <v>45246</v>
+        <v>45268</v>
       </c>
       <c r="D135" s="40"/>
       <c r="E135" s="43"/>
-      <c r="F135" s="69" t="s">
+      <c r="F135" s="66" t="s">
         <v>195</v>
       </c>
-      <c r="G135" s="70" t="s">
+      <c r="G135" s="67" t="s">
         <v>196</v>
       </c>
-      <c r="H135" s="70"/>
-      <c r="I135" s="69" t="s">
+      <c r="H135" s="67"/>
+      <c r="I135" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="J135" s="69" t="s">
+      <c r="J135" s="66" t="s">
         <v>156</v>
       </c>
       <c r="K135" s="62" t="s">
@@ -7685,7 +7736,7 @@
       </c>
     </row>
     <row r="161" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A161" s="68">
+      <c r="A161" s="65">
         <v>160</v>
       </c>
       <c r="B161" s="38">
@@ -13401,6 +13452,141 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCD2CC7-9F91-4396-B657-29A3F12280C4}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="77">
+        <v>1</v>
+      </c>
+      <c r="B2" s="71" t="s">
+        <v>263</v>
+      </c>
+      <c r="C2" s="72"/>
+      <c r="D2" s="73" t="s">
+        <v>264</v>
+      </c>
+      <c r="E2" s="74" t="s">
+        <v>194</v>
+      </c>
+      <c r="F2" s="74"/>
+      <c r="G2" s="73" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="73" t="s">
+        <v>156</v>
+      </c>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+    </row>
+    <row r="3" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="78">
+        <v>2</v>
+      </c>
+      <c r="B3" s="76"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="73" t="s">
+        <v>195</v>
+      </c>
+      <c r="E3" s="74" t="s">
+        <v>196</v>
+      </c>
+      <c r="F3" s="74"/>
+      <c r="G3" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="73" t="s">
+        <v>156</v>
+      </c>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="71" t="s">
+        <v>261</v>
+      </c>
+      <c r="C4" s="79"/>
+      <c r="D4" s="75" t="s">
+        <v>258</v>
+      </c>
+      <c r="E4" s="80" t="s">
+        <v>262</v>
+      </c>
+      <c r="F4" s="80"/>
+      <c r="G4" s="75" t="s">
+        <v>259</v>
+      </c>
+      <c r="H4" s="75" t="s">
+        <v>209</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H4" xr:uid="{66CBD4FF-22E1-4D8C-B1ED-421CBC96ECA0}">
+      <formula1>"Rahul Dutta,Just Dial,Anirban Chakraborty"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E2:E3" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF1703B3-076E-40BB-A643-6D0582148E8C}">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -13419,15 +13605,15 @@
       <c r="A1" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="68" t="s">
         <v>252</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="67"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="70"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="13">

</xml_diff>

<commit_message>
Enquiry and To Do List updated
Enquiry and To Do List updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/CRM/Enquiry.xlsx
+++ b/Offline/BusinessManagement/CRM/Enquiry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\CRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5F71A5-C58B-4D72-8786-ECBE5A31F118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33877DE0-7AAB-4C2C-B032-101367994425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="437" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,7 +522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="318">
   <si>
     <t>Student Name</t>
   </si>
@@ -1482,7 +1482,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1512,6 +1512,13 @@
     <font>
       <sz val="10"/>
       <name val="Oxygen"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1634,7 +1641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1807,9 +1814,6 @@
     <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1822,6 +1826,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2307,9 +2331,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O494"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O158" sqref="O158"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C160" sqref="C160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6746,34 +6770,34 @@
       <c r="B133" s="57">
         <v>45246</v>
       </c>
-      <c r="C133" s="57">
+      <c r="C133" s="59">
         <v>45246</v>
       </c>
-      <c r="D133" s="58"/>
-      <c r="E133" s="56"/>
-      <c r="F133" s="56" t="s">
+      <c r="D133" s="62"/>
+      <c r="E133" s="61"/>
+      <c r="F133" s="61" t="s">
         <v>192</v>
       </c>
-      <c r="G133" s="24" t="s">
+      <c r="G133" s="67" t="s">
         <v>193</v>
       </c>
-      <c r="H133" s="24"/>
-      <c r="I133" s="8" t="s">
+      <c r="H133" s="67"/>
+      <c r="I133" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="J133" s="8" t="s">
+      <c r="J133" s="66" t="s">
         <v>156</v>
       </c>
-      <c r="K133" s="58" t="s">
+      <c r="K133" s="62" t="s">
         <v>200</v>
       </c>
-      <c r="L133" s="58"/>
-      <c r="M133" s="58"/>
-      <c r="N133" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="O133" s="58" t="s">
-        <v>250</v>
+      <c r="L133" s="62"/>
+      <c r="M133" s="62"/>
+      <c r="N133" s="41" t="s">
+        <v>205</v>
+      </c>
+      <c r="O133" s="62" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.3">
@@ -7677,7 +7701,9 @@
       <c r="B160" s="38">
         <v>45268</v>
       </c>
-      <c r="C160" s="39"/>
+      <c r="C160" s="38">
+        <v>45268</v>
+      </c>
       <c r="D160" s="40" t="s">
         <v>315</v>
       </c>
@@ -13423,25 +13449,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCD2CC7-9F91-4396-B657-29A3F12280C4}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
     <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="10" max="10" width="28.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>103</v>
       </c>
@@ -13473,8 +13498,8 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="68">
+    <row r="2" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="75">
         <v>1</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -13498,7 +13523,7 @@
       <c r="J2" s="58"/>
     </row>
     <row r="3" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+      <c r="A3" s="76">
         <v>2</v>
       </c>
       <c r="B3" s="17"/>
@@ -13520,7 +13545,7 @@
       <c r="J3" s="58"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+      <c r="A4" s="76">
         <v>3</v>
       </c>
       <c r="B4" s="25" t="s">
@@ -13530,18 +13555,40 @@
       <c r="D4" s="58" t="s">
         <v>258</v>
       </c>
-      <c r="E4" s="69" t="s">
+      <c r="E4" s="68" t="s">
         <v>262</v>
       </c>
-      <c r="F4" s="69"/>
+      <c r="F4" s="68"/>
       <c r="G4" s="58" t="s">
         <v>259</v>
       </c>
       <c r="H4" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="78">
+        <v>4</v>
+      </c>
+      <c r="B5" s="72"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73" t="s">
+        <v>192</v>
+      </c>
+      <c r="E5" s="74" t="s">
+        <v>193</v>
+      </c>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="79" t="s">
+        <v>156</v>
+      </c>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -13575,15 +13622,15 @@
       <c r="A1" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="69" t="s">
         <v>252</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="72"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="71"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="13">

</xml_diff>

<commit_message>
Enquiry and Faculty List updated
Enquiry and Faculty List updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/CRM/Enquiry.xlsx
+++ b/Offline/BusinessManagement/CRM/Enquiry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\CRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33877DE0-7AAB-4C2C-B032-101367994425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CD1337-EF23-443F-A354-247080B254E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="437" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="437" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prospects" sheetId="2" r:id="rId1"/>
@@ -1482,7 +1482,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1512,13 +1512,6 @@
     <font>
       <sz val="10"/>
       <name val="Oxygen"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1641,7 +1634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1826,26 +1819,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2331,7 +2307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O494"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C160" sqref="C160"/>
     </sheetView>
@@ -13449,9 +13425,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCD2CC7-9F91-4396-B657-29A3F12280C4}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -13499,7 +13477,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="75">
+      <c r="A2" s="72">
         <v>1</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -13523,7 +13501,7 @@
       <c r="J2" s="58"/>
     </row>
     <row r="3" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="76">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
       <c r="B3" s="17"/>
@@ -13545,7 +13523,7 @@
       <c r="J3" s="58"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="76">
+      <c r="A4" s="23">
         <v>3</v>
       </c>
       <c r="B4" s="25" t="s">
@@ -13565,30 +13543,606 @@
       <c r="H4" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="78">
+      <c r="A5" s="23">
         <v>4</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73" t="s">
+      <c r="B5" s="58"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56" t="s">
         <v>192</v>
       </c>
-      <c r="E5" s="74" t="s">
+      <c r="E5" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79" t="s">
+      <c r="F5" s="15"/>
+      <c r="G5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="79" t="s">
+      <c r="H5" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="28"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="28"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="28"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="28"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="28"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="28"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="28"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="28"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="28"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="28"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="28"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="28"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="28"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="28"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="28"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="28"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="28"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="28"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="28"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="28"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="28"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="29"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="28"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="28"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="28"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="29"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="29"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="28"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="29"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="28"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="28"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="29"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="28"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="29"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="28"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
+      <c r="J53" s="29"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
To do list and speakers list added
To do list and speakers list added
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/CRM/Enquiry.xlsx
+++ b/Offline/BusinessManagement/CRM/Enquiry.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\CRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA99297-2A78-43D0-9C28-8F1B9D519912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43367E20-5226-4C08-B848-07E8F70A1234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="437" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="534" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prospects" sheetId="2" r:id="rId1"/>
-    <sheet name="Demo-16-12-2023" sheetId="8" r:id="rId2"/>
-    <sheet name="Notes" sheetId="7" r:id="rId3"/>
+    <sheet name="ToDoList-16-12-2023" sheetId="9" r:id="rId2"/>
+    <sheet name="Students-For-Demo-16-12-2023" sheetId="8" r:id="rId3"/>
+    <sheet name="Speakers" sheetId="11" r:id="rId4"/>
+    <sheet name="Notes" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Prospects!$A$1:$O$159</definedName>
@@ -522,7 +524,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="360">
   <si>
     <t>Student Name</t>
   </si>
@@ -1476,6 +1478,132 @@
   </si>
   <si>
     <t>Sreya Naskar</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Call Bappa for discussion of demo on 16-12-2023</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>He will come on 10-12-2023 at 11:00 AM</t>
+  </si>
+  <si>
+    <t>Get a maid for cleaning the demo room</t>
+  </si>
+  <si>
+    <t>Not-Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clean the demo room on the 2nd floor </t>
+  </si>
+  <si>
+    <t>Make a separate list of students for demo</t>
+  </si>
+  <si>
+    <t>In-Progress</t>
+  </si>
+  <si>
+    <t>3 sudents has been listed</t>
+  </si>
+  <si>
+    <t>Get the different accessories like table or chair to decorate the room for demo</t>
+  </si>
+  <si>
+    <t>Rahul needed to call gurdian Madhuparna acharya to confirm.</t>
+  </si>
+  <si>
+    <t>Keep the toys and other accessories inside the demo room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make the required signages for demo room </t>
+  </si>
+  <si>
+    <t>Install the CCTV camera inside the demo room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paste different posters for children in the demo room </t>
+  </si>
+  <si>
+    <t>We have 2 posters.</t>
+  </si>
+  <si>
+    <t>Paste different posters for children in the stair case</t>
+  </si>
+  <si>
+    <t>Paste posters in the entrance for demo date 16 Dec 2023</t>
+  </si>
+  <si>
+    <t>Place a standie in the entrance for demo date 16 Dec 2023</t>
+  </si>
+  <si>
+    <t>Make a stock for tea,coffee,buiscuits and choclates for demo date 16 Dec 2023</t>
+  </si>
+  <si>
+    <t>Complete the anodiam website</t>
+  </si>
+  <si>
+    <t>Deploy the anodiam website</t>
+  </si>
+  <si>
+    <t>Fix the green screen in front of the racks</t>
+  </si>
+  <si>
+    <t>Call Hiya for 16th Dec demo</t>
+  </si>
+  <si>
+    <t>Fix the TV</t>
+  </si>
+  <si>
+    <t>Fix the white board in the demo room for 16 Dec 2023</t>
+  </si>
+  <si>
+    <t>Speakers</t>
+  </si>
+  <si>
+    <t>AI/ML Foundation</t>
+  </si>
+  <si>
+    <t>Coding Core</t>
+  </si>
+  <si>
+    <t>Topics</t>
+  </si>
+  <si>
+    <t>Bappaditto</t>
+  </si>
+  <si>
+    <t>Robotics</t>
+  </si>
+  <si>
+    <t>IOT</t>
+  </si>
+  <si>
+    <t>Vedic Maths</t>
+  </si>
+  <si>
+    <t>Mental Maths</t>
+  </si>
+  <si>
+    <t>Communication Skills</t>
+  </si>
+  <si>
+    <t>Social Intelligence</t>
+  </si>
+  <si>
+    <t>Avishek Adhikari</t>
+  </si>
+  <si>
+    <t>Sayan Basak</t>
+  </si>
+  <si>
+    <t>Srijina Mukherjee</t>
   </si>
 </sst>
 </file>
@@ -1634,7 +1762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1822,6 +1950,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2307,7 +2439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O494"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A133" sqref="A133:B133"/>
     </sheetView>
@@ -13424,6 +13556,278 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045D750C-437C-4FDE-8711-D29AC39547FA}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="73" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>318</v>
+      </c>
+      <c r="C1" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="74" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>326</v>
+      </c>
+      <c r="C6" t="s">
+        <v>327</v>
+      </c>
+      <c r="D6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>329</v>
+      </c>
+      <c r="C7" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>330</v>
+      </c>
+      <c r="C8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>331</v>
+      </c>
+      <c r="C9" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>332</v>
+      </c>
+      <c r="C10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>333</v>
+      </c>
+      <c r="C11" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>334</v>
+      </c>
+      <c r="C12" t="s">
+        <v>324</v>
+      </c>
+      <c r="D12" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>336</v>
+      </c>
+      <c r="C13" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>337</v>
+      </c>
+      <c r="C14" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>338</v>
+      </c>
+      <c r="C15" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>339</v>
+      </c>
+      <c r="C16" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>340</v>
+      </c>
+      <c r="C17" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>341</v>
+      </c>
+      <c r="C18" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>342</v>
+      </c>
+      <c r="C19" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>343</v>
+      </c>
+      <c r="C20" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>344</v>
+      </c>
+      <c r="C21" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>345</v>
+      </c>
+      <c r="C22" t="s">
+        <v>321</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C22" xr:uid="{68EC632A-C1DC-4AE5-809B-998D1ADAD475}">
+      <formula1>"Done,Not-Done,In-Progress"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCD2CC7-9F91-4396-B657-29A3F12280C4}">
   <dimension ref="A1:J53"/>
   <sheetViews>
@@ -14157,7 +14561,102 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4DD6C2-234E-4F52-95E8-21E397410B80}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="73" t="s">
+        <v>251</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1" s="74" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>350</v>
+      </c>
+      <c r="C6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>357</v>
+      </c>
+      <c r="C9" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>359</v>
+      </c>
+      <c r="C12" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>356</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF1703B3-076E-40BB-A643-6D0582148E8C}">
   <dimension ref="A1:H11"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated Enquiry and Ops for Dec 2023
Updated Enquiry and Ops for Dec 2023
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/CRM/Enquiry.xlsx
+++ b/Offline/BusinessManagement/CRM/Enquiry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\CRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263D59B2-608D-46FE-BBCB-DFB8A8E1623B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993B3158-B1BD-4CC3-A8B0-E1FD333B4800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="534" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2068,6 +2068,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2076,9 +2079,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -14708,7 +14708,7 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14737,7 +14737,7 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="E1" s="71" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="5" t="s">
@@ -15620,15 +15620,15 @@
       <c r="A1" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="72" t="s">
         <v>251</v>
       </c>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="74"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="13">

</xml_diff>

<commit_message>
Updated CRM sheet. Created a new sheet Requirement-Analysis for AI courses
Updated CRM sheet. Created a new sheet Requirement-Analysis for AI courses
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/CRM/Enquiry.xlsx
+++ b/Offline/BusinessManagement/CRM/Enquiry.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\CRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4C64E4-869B-40AD-A4BE-3C04DA7A1CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B361C1F1-F23A-4C49-9D5A-B19EEB175B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="666" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prospects" sheetId="2" r:id="rId1"/>
-    <sheet name="ToDoList-16-12-2023" sheetId="9" r:id="rId2"/>
-    <sheet name="Expense-For-16-12-2023" sheetId="13" r:id="rId3"/>
-    <sheet name="Students-For-Demo-16-12-2023" sheetId="8" r:id="rId4"/>
-    <sheet name="Speakers-16-12-2023" sheetId="11" r:id="rId5"/>
-    <sheet name="Mock-Test" sheetId="12" r:id="rId6"/>
+    <sheet name="Mock-Test" sheetId="12" r:id="rId2"/>
+    <sheet name="ToDoList-16-12-2023" sheetId="9" r:id="rId3"/>
+    <sheet name="Expense-For-16-12-2023" sheetId="13" r:id="rId4"/>
+    <sheet name="Students-For-Demo-16-12-2023" sheetId="8" r:id="rId5"/>
+    <sheet name="Speakers-16-12-2023" sheetId="11" r:id="rId6"/>
     <sheet name="Notes" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Prospects!$A$1:$Q$170</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ToDoList-16-12-2023'!$A$1:$D$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ToDoList-16-12-2023'!$A$1:$D$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -102,6 +102,7 @@
     <author>tc={1483095E-DA2F-4796-815F-70FAE56732AA}</author>
     <author>tc={9CC0344F-B0BC-4CF9-A879-66E1F7D11D86}</author>
     <author>tc={DD18A624-EE4D-4397-9F42-805F236BF3AA}</author>
+    <author>tc={871D56C2-4972-4DB0-A6F7-F334C8FA3A28}</author>
   </authors>
   <commentList>
     <comment ref="N62" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -618,12 +619,21 @@
 We need to send course details with fees.</t>
       </text>
     </comment>
+    <comment ref="N173" authorId="56" shapeId="0" xr:uid="{871D56C2-4972-4DB0-A6F7-F334C8FA3A28}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    She is house wife.
+</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="418">
   <si>
     <t>Student Name</t>
   </si>
@@ -1874,6 +1884,9 @@
   </si>
   <si>
     <t>BTech 3rd Year</t>
+  </si>
+  <si>
+    <t>Swati</t>
   </si>
 </sst>
 </file>
@@ -1915,7 +1928,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2766,6 +2779,10 @@
     <text>She is studying BTech (3rd Year) .
 We need to send course details with fees.</text>
   </threadedComment>
+  <threadedComment ref="N173" dT="2023-12-18T06:20:05.19" personId="{4666E732-BD10-4E5E-A636-505584664154}" id="{871D56C2-4972-4DB0-A6F7-F334C8FA3A28}">
+    <text xml:space="preserve">She is house wife.
+</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2774,9 +2791,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q494"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N176" sqref="N176"/>
+      <selection pane="bottomLeft" activeCell="N173" sqref="N173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8910,7 +8927,9 @@
       <c r="B171" s="20">
         <v>45275</v>
       </c>
-      <c r="C171" s="15"/>
+      <c r="C171" s="20">
+        <v>45277</v>
+      </c>
       <c r="D171" s="15"/>
       <c r="E171" s="17"/>
       <c r="F171" s="18"/>
@@ -8949,7 +8968,9 @@
       <c r="B172" s="20">
         <v>45276</v>
       </c>
-      <c r="C172" s="15"/>
+      <c r="C172" s="20">
+        <v>45276</v>
+      </c>
       <c r="D172" s="15"/>
       <c r="E172" s="17" t="s">
         <v>414</v>
@@ -8980,23 +9001,41 @@
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A173" s="23"/>
-      <c r="B173" s="15"/>
+      <c r="A173" s="23">
+        <v>172</v>
+      </c>
+      <c r="B173" s="20">
+        <v>45277</v>
+      </c>
       <c r="C173" s="15"/>
       <c r="D173" s="15"/>
-      <c r="E173" s="17"/>
-      <c r="F173" s="18"/>
+      <c r="E173" s="30" t="s">
+        <v>417</v>
+      </c>
+      <c r="F173" s="17">
+        <v>7992263185</v>
+      </c>
       <c r="G173" s="15"/>
       <c r="H173" s="22"/>
       <c r="I173" s="19"/>
-      <c r="J173" s="15"/>
-      <c r="K173" s="15"/>
-      <c r="L173" s="17"/>
+      <c r="J173" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="K173" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="L173" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="M173" s="17"/>
       <c r="N173" s="15"/>
-      <c r="O173" s="16"/>
+      <c r="O173" s="16" t="s">
+        <v>204</v>
+      </c>
       <c r="P173" s="16"/>
-      <c r="Q173" s="15"/>
+      <c r="Q173" s="15" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A174" s="23"/>
@@ -15126,1363 +15165,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="93.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>317</v>
-      </c>
-      <c r="C1" s="69" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="69" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>321</v>
-      </c>
-      <c r="C3" t="s">
-        <v>320</v>
-      </c>
-      <c r="D3" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>323</v>
-      </c>
-      <c r="C4" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>324</v>
-      </c>
-      <c r="C5" t="s">
-        <v>320</v>
-      </c>
-      <c r="D5" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>326</v>
-      </c>
-      <c r="C6" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>327</v>
-      </c>
-      <c r="C7" t="s">
-        <v>320</v>
-      </c>
-      <c r="D7" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>328</v>
-      </c>
-      <c r="C8" t="s">
-        <v>322</v>
-      </c>
-      <c r="D8" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>329</v>
-      </c>
-      <c r="C9" t="s">
-        <v>322</v>
-      </c>
-      <c r="D9" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>330</v>
-      </c>
-      <c r="C10" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>331</v>
-      </c>
-      <c r="C11" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>332</v>
-      </c>
-      <c r="C12" t="s">
-        <v>322</v>
-      </c>
-      <c r="D12" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>358</v>
-      </c>
-      <c r="C13" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>333</v>
-      </c>
-      <c r="C14" t="s">
-        <v>325</v>
-      </c>
-      <c r="D14" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>334</v>
-      </c>
-      <c r="C15" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>335</v>
-      </c>
-      <c r="C16" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>336</v>
-      </c>
-      <c r="C17" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>337</v>
-      </c>
-      <c r="C18" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>405</v>
-      </c>
-      <c r="C19" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>361</v>
-      </c>
-      <c r="C20" t="s">
-        <v>325</v>
-      </c>
-      <c r="D20" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>362</v>
-      </c>
-      <c r="C21" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>363</v>
-      </c>
-      <c r="C22" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>410</v>
-      </c>
-      <c r="C23" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>408</v>
-      </c>
-      <c r="C24" t="s">
-        <v>322</v>
-      </c>
-      <c r="D24" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>367</v>
-      </c>
-      <c r="C25" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>406</v>
-      </c>
-      <c r="C26" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>407</v>
-      </c>
-      <c r="C27" t="s">
-        <v>325</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:D27" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
-      <formula1>"Done,Not-Done,In-Progress"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AB0DC1-1F50-4EDD-8833-E2ED2FCD27C5}">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="B1" s="77" t="s">
-        <v>399</v>
-      </c>
-      <c r="C1" s="77" t="s">
-        <v>400</v>
-      </c>
-      <c r="D1" s="69"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>401</v>
-      </c>
-      <c r="C3" s="11">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>404</v>
-      </c>
-      <c r="C4" s="11">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>403</v>
-      </c>
-      <c r="C5" s="11">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
-        <v>4</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>412</v>
-      </c>
-      <c r="C6" s="11">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="77" t="s">
-        <v>413</v>
-      </c>
-      <c r="C8" s="77">
-        <f>SUM(C3:C6)</f>
-        <v>2600</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J53"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="70" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="67">
-        <v>1</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>262</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-    </row>
-    <row r="3" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23">
-        <v>2</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="67">
-        <v>3</v>
-      </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56" t="s">
-        <v>191</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="23">
-        <v>4</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="C5" s="15">
-        <v>8336817657</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="67">
-        <v>5</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="17">
-        <v>7278448048</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="23">
-        <v>6</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="15" t="s">
-        <v>293</v>
-      </c>
-      <c r="E7" s="17">
-        <v>9830826860</v>
-      </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="67">
-        <v>7</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C8" s="15">
-        <v>6294268223</v>
-      </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="23">
-        <v>8</v>
-      </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="15" t="s">
-        <v>373</v>
-      </c>
-      <c r="E9" s="17">
-        <v>9433055625</v>
-      </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="67">
-        <v>9</v>
-      </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="E10" s="17">
-        <v>8016981657</v>
-      </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="23">
-        <v>10</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="C11" s="15">
-        <v>7596825771</v>
-      </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="23">
-        <v>11</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>374</v>
-      </c>
-      <c r="C12" s="15">
-        <v>7596825771</v>
-      </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="28"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="28"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="28"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="28"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="28"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="28"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="28"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="28"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="28"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="28"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="28"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="28"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="28"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="28"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="28"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="28"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="28"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="29"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="28"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
-      <c r="J35" s="29"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="28"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
-      <c r="J36" s="29"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="28"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="28"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="28"/>
-      <c r="B39" s="29"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="29"/>
-      <c r="J39" s="29"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="28"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="28"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="29"/>
-      <c r="J41" s="29"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="28"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="28"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="28"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="28"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="29"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="28"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="29"/>
-      <c r="H46" s="29"/>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="28"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="29"/>
-      <c r="J47" s="29"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" s="28"/>
-      <c r="B48" s="29"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="29"/>
-      <c r="H48" s="29"/>
-      <c r="I48" s="29"/>
-      <c r="J48" s="29"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="28"/>
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="29"/>
-      <c r="I49" s="29"/>
-      <c r="J49" s="29"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="28"/>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="29"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="28"/>
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="29"/>
-      <c r="H51" s="29"/>
-      <c r="I51" s="29"/>
-      <c r="J51" s="29"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" s="28"/>
-      <c r="B52" s="29"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="29"/>
-      <c r="H52" s="29"/>
-      <c r="I52" s="29"/>
-      <c r="J52" s="29"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53" s="28"/>
-      <c r="B53" s="29"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="29"/>
-      <c r="H53" s="29"/>
-      <c r="I53" s="29"/>
-      <c r="J53" s="29"/>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H3" xr:uid="{00000000-0002-0000-0200-000000000000}">
-      <formula1>"Rahul Dutta,Just Dial,Anirban Chakraborty"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="E2:E3" numberStoredAsText="1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
-        <v>250</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>338</v>
-      </c>
-      <c r="C1" s="69" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>350</v>
-      </c>
-      <c r="C3" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>342</v>
-      </c>
-      <c r="C6" t="s">
-        <v>343</v>
-      </c>
-      <c r="D6" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>344</v>
-      </c>
-      <c r="D7" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>349</v>
-      </c>
-      <c r="C9" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>351</v>
-      </c>
-      <c r="C12" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>208</v>
-      </c>
-      <c r="C15" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA3EFE6-3859-4192-80B3-DA69B1417FF7}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -16628,6 +15310,1363 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="93.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>317</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C3" t="s">
+        <v>320</v>
+      </c>
+      <c r="D3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>324</v>
+      </c>
+      <c r="C5" t="s">
+        <v>320</v>
+      </c>
+      <c r="D5" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>326</v>
+      </c>
+      <c r="C6" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>327</v>
+      </c>
+      <c r="C7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D7" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>328</v>
+      </c>
+      <c r="C8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D8" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>329</v>
+      </c>
+      <c r="C9" t="s">
+        <v>322</v>
+      </c>
+      <c r="D9" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>330</v>
+      </c>
+      <c r="C10" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>331</v>
+      </c>
+      <c r="C11" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>332</v>
+      </c>
+      <c r="C12" t="s">
+        <v>322</v>
+      </c>
+      <c r="D12" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>358</v>
+      </c>
+      <c r="C13" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>333</v>
+      </c>
+      <c r="C14" t="s">
+        <v>325</v>
+      </c>
+      <c r="D14" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>334</v>
+      </c>
+      <c r="C15" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>335</v>
+      </c>
+      <c r="C16" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>336</v>
+      </c>
+      <c r="C17" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>337</v>
+      </c>
+      <c r="C18" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>405</v>
+      </c>
+      <c r="C19" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>361</v>
+      </c>
+      <c r="C20" t="s">
+        <v>325</v>
+      </c>
+      <c r="D20" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>362</v>
+      </c>
+      <c r="C21" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>363</v>
+      </c>
+      <c r="C22" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>410</v>
+      </c>
+      <c r="C23" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>408</v>
+      </c>
+      <c r="C24" t="s">
+        <v>322</v>
+      </c>
+      <c r="D24" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>367</v>
+      </c>
+      <c r="C25" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>406</v>
+      </c>
+      <c r="C26" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>407</v>
+      </c>
+      <c r="C27" t="s">
+        <v>325</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D27" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+      <formula1>"Done,Not-Done,In-Progress"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AB0DC1-1F50-4EDD-8833-E2ED2FCD27C5}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="77" t="s">
+        <v>399</v>
+      </c>
+      <c r="C1" s="77" t="s">
+        <v>400</v>
+      </c>
+      <c r="D1" s="69"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>401</v>
+      </c>
+      <c r="C3" s="11">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>404</v>
+      </c>
+      <c r="C4" s="11">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>403</v>
+      </c>
+      <c r="C5" s="11">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="C6" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="77" t="s">
+        <v>413</v>
+      </c>
+      <c r="C8" s="77">
+        <f>SUM(C3:C6)</f>
+        <v>2600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="67">
+        <v>1</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+    </row>
+    <row r="3" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="23">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="F3" s="24"/>
+      <c r="G3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="67">
+        <v>3</v>
+      </c>
+      <c r="B4" s="58"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="23">
+        <v>4</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="15">
+        <v>8336817657</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="67">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="17">
+        <v>7278448048</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="23">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="E7" s="17">
+        <v>9830826860</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="67">
+        <v>7</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="15">
+        <v>6294268223</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="23">
+        <v>8</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="E9" s="17">
+        <v>9433055625</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="67">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" s="17">
+        <v>8016981657</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="23">
+        <v>10</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="15">
+        <v>7596825771</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="23">
+        <v>11</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>374</v>
+      </c>
+      <c r="C12" s="15">
+        <v>7596825771</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="28"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="28"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="28"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="28"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="28"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="28"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="28"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="28"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="28"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="28"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="28"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="28"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="28"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="28"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="28"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="28"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="28"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="28"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="28"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="28"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="28"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="29"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="28"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="28"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="28"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="29"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="29"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="28"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="29"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="28"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="28"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="29"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="28"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="29"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="28"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
+      <c r="J53" s="29"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H3" xr:uid="{00000000-0002-0000-0200-000000000000}">
+      <formula1>"Rahul Dutta,Just Dial,Anirban Chakraborty"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E2:E3" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="68" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>338</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C3" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>342</v>
+      </c>
+      <c r="C6" t="s">
+        <v>343</v>
+      </c>
+      <c r="D6" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>344</v>
+      </c>
+      <c r="D7" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>349</v>
+      </c>
+      <c r="C9" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>351</v>
+      </c>
+      <c r="C12" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>208</v>
+      </c>
+      <c r="C15" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>348</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H11"/>

</xml_diff>

<commit_message>
Update Enquiry with 1 mock test student
Update Enquiry with 1 mock test student
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/CRM/Enquiry.xlsx
+++ b/Offline/BusinessManagement/CRM/Enquiry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\CRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3673B6-17B5-444B-9D2D-51B03F74236A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D120D5-A772-40C3-8371-52111FE86A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" tabRatio="535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="535" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prospects" sheetId="2" r:id="rId1"/>
@@ -103,6 +103,7 @@
     <author>tc={9CC0344F-B0BC-4CF9-A879-66E1F7D11D86}</author>
     <author>tc={DD18A624-EE4D-4397-9F42-805F236BF3AA}</author>
     <author>tc={871D56C2-4972-4DB0-A6F7-F334C8FA3A28}</author>
+    <author>tc={697E72CD-BAF4-4A69-8506-8ADA49700B8B}</author>
   </authors>
   <commentList>
     <comment ref="N62" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -630,12 +631,26 @@
 She will come on 19-12-2023 at 4 PM.</t>
       </text>
     </comment>
+    <comment ref="N174" authorId="57" shapeId="0" xr:uid="{697E72CD-BAF4-4A69-8506-8ADA49700B8B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Her son will give mock test exam on 5 subjects
+Accountancy
+Business Studies
+English
+Maths
+Economics
+We need to give her the time table</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="425">
   <si>
     <t>Student Name</t>
   </si>
@@ -1892,13 +1907,31 @@
   </si>
   <si>
     <t>Priyankshu Giri</t>
+  </si>
+  <si>
+    <t>Accountancy</t>
+  </si>
+  <si>
+    <t>Ritayan Paul</t>
+  </si>
+  <si>
+    <t>Arpita Paul</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>Business Studies</t>
+  </si>
+  <si>
+    <t>CBSE Std XII</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1928,6 +1961,12 @@
     <font>
       <sz val="10"/>
       <name val="Oxygen"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2050,7 +2089,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2260,6 +2299,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2787,6 +2832,15 @@
     <text>She is house wife.
 She will come on 19-12-2023 at 4 PM.</text>
   </threadedComment>
+  <threadedComment ref="N174" dT="2023-12-18T11:20:08.88" personId="{4666E732-BD10-4E5E-A636-505584664154}" id="{697E72CD-BAF4-4A69-8506-8ADA49700B8B}">
+    <text>Her son will give mock test exam on 5 subjects
+Accountancy
+Business Studies
+English
+Maths
+Economics
+We need to give her the time table</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2795,9 +2849,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q494"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E171" sqref="E171"/>
+      <selection pane="bottomLeft" activeCell="M174" sqref="M174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9050,23 +9104,41 @@
       </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A174" s="23"/>
+      <c r="A174" s="23">
+        <v>173</v>
+      </c>
       <c r="B174" s="15"/>
       <c r="C174" s="15"/>
       <c r="D174" s="15"/>
-      <c r="E174" s="17"/>
-      <c r="F174" s="18"/>
-      <c r="G174" s="15"/>
-      <c r="H174" s="22"/>
+      <c r="E174" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="F174" s="11"/>
+      <c r="G174" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="H174" s="82">
+        <v>9007505027</v>
+      </c>
       <c r="I174" s="19"/>
       <c r="J174" s="15"/>
       <c r="K174" s="15"/>
-      <c r="L174" s="17"/>
-      <c r="M174" s="17"/>
+      <c r="L174" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="M174" s="17" t="s">
+        <v>299</v>
+      </c>
       <c r="N174" s="15"/>
-      <c r="O174" s="16"/>
-      <c r="P174" s="16"/>
-      <c r="Q174" s="15"/>
+      <c r="O174" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="P174" s="83">
+        <v>45290</v>
+      </c>
+      <c r="Q174" s="15" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A175" s="23"/>
@@ -15178,10 +15250,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA3EFE6-3859-4192-80B3-DA69B1417FF7}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15190,17 +15262,17 @@
     <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.21875" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.88671875" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>103</v>
       </c>
@@ -15223,22 +15295,25 @@
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="76" t="s">
+      <c r="K1" s="76" t="s">
         <v>392</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -15258,21 +15333,22 @@
         <v>253</v>
       </c>
       <c r="G2" s="18"/>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="18"/>
+      <c r="I2" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="I2" s="73">
+      <c r="J2" s="73">
         <v>8777380801</v>
       </c>
-      <c r="J2" s="73" t="s">
+      <c r="K2" s="73" t="s">
         <v>208</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>385</v>
       </c>
-      <c r="L2" s="11"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2" s="11"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -15292,30 +15368,198 @@
         <v>253</v>
       </c>
       <c r="G3" s="18"/>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="18"/>
+      <c r="I3" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="I3" s="73">
+      <c r="J3" s="73">
         <v>8777380801</v>
       </c>
-      <c r="J3" s="73" t="s">
+      <c r="K3" s="73" t="s">
         <v>208</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="L3" s="11" t="s">
         <v>385</v>
       </c>
-      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="74">
+        <v>45290</v>
+      </c>
+      <c r="C4" s="75">
+        <v>0.4375</v>
+      </c>
+      <c r="D4" s="75">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="J4" s="82">
+        <v>9007505027</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="M4" s="11"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="74"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>423</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="J5" s="82">
+        <v>9007505027</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="M5" s="11"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="74">
+        <v>45290</v>
+      </c>
+      <c r="C6" s="75">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D6" s="75">
+        <v>0.6875</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="J6" s="82">
+        <v>9007505027</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="74"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="J7" s="82">
+        <v>9007505027</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="M7" s="11"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="74"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="J8" s="82">
+        <v>9007505027</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="M8" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576" xr:uid="{76AB7963-4243-4657-8766-5DBD81C38EC2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576" xr:uid="{76AB7963-4243-4657-8766-5DBD81C38EC2}">
       <formula1>"Appeared,Not-Appeared,Enrolled"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576" xr:uid="{033DCDB4-449D-4568-91C0-6B18E5A7E402}">
-      <formula1>"Rahul Dutta"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576" xr:uid="{033DCDB4-449D-4568-91C0-6B18E5A7E402}">
+      <formula1>"Rahul Dutta,Anupam Sen"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{4F6B866F-5D56-46D4-AC31-3565050B0508}">
-      <formula1>"English,Bengali,Geography,Maths"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{8629B26E-F5E8-4B8B-BD4D-E9647B5A1EB4}">
+      <formula1>"English,Geography,Accountancy,Business Studies,Maths,Economics"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>